<commit_message>
Updated params Q0005, Q0006 and P0027 with info html
</commit_message>
<xml_diff>
--- a/paramData Excels/Q0005.xlsx
+++ b/paramData Excels/Q0005.xlsx
@@ -1,211 +1,333 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="R1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Param item
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>is the item already used in the table?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">item name in dated param P0050
+(e-g) P0050 is param; item could be FREQ, BCUR
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>[4]string</t>
+  </si>
+  <si>
+    <t>[]string</t>
+  </si>
   <si>
     <t>COLUMN_KEY</t>
   </si>
   <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>COLUMN_NAME</t>
+  </si>
+  <si>
+    <t>DATA_TYPE</t>
+  </si>
+  <si>
+    <t>CHARACTER_MAXIMUM_LENGTH</t>
+  </si>
+  <si>
+    <t>NUMERIC_PRECISION</t>
+  </si>
+  <si>
+    <t>DATETIME_PRECISION</t>
+  </si>
+  <si>
+    <t>IS_NULLABLE</t>
+  </si>
+  <si>
+    <t>Column Description</t>
+  </si>
+  <si>
+    <t>Add_flag</t>
+  </si>
+  <si>
+    <t>Edit_flag</t>
+  </si>
+  <si>
+    <t>Info_flag</t>
+  </si>
+  <si>
+    <t>Grid_flag</t>
+  </si>
+  <si>
+    <t>param</t>
+  </si>
+  <si>
+    <t>lookup_table</t>
+  </si>
+  <si>
+    <t>ORDINAL_POSITION</t>
+  </si>
+  <si>
     <t>PARAM_NAME</t>
   </si>
   <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>COLUMN_NAME</t>
-  </si>
-  <si>
-    <t>DATA_TYPE</t>
-  </si>
-  <si>
-    <t>CHARACTER_MAXIMUM_LENGTH</t>
-  </si>
-  <si>
-    <t>NUMERIC_PRECISION</t>
-  </si>
-  <si>
-    <t>DATETIME_PRECISION</t>
-  </si>
-  <si>
-    <t>IS_NULLABLE</t>
-  </si>
-  <si>
-    <t>Column Description</t>
-  </si>
-  <si>
-    <t>Add_flag</t>
-  </si>
-  <si>
-    <t>Edit_flag</t>
-  </si>
-  <si>
-    <t>Info_flag</t>
-  </si>
-  <si>
-    <t>Grid_flag</t>
-  </si>
-  <si>
-    <t>param</t>
-  </si>
-  <si>
-    <t>lookup_table</t>
+    <t>Q0005</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Free look Days</t>
+  </si>
+  <si>
+    <t>Maximum Lives</t>
+  </si>
+  <si>
+    <t>Minimum Lives</t>
+  </si>
+  <si>
+    <t>Product  Family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renewable  </t>
+  </si>
+  <si>
+    <t>Allowable Frequencies</t>
+  </si>
+  <si>
+    <t>Contract Currency</t>
+  </si>
+  <si>
+    <t>Billing Currency</t>
+  </si>
+  <si>
+    <t>Min.period for Surrender (in months)</t>
+  </si>
+  <si>
+    <t>Reinstatement from PTD (in months)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>MaxLives</t>
+  </si>
+  <si>
+    <t>FreeLookDays</t>
+  </si>
+  <si>
+    <t>MinLives</t>
+  </si>
+  <si>
+    <t>ProductFamily</t>
+  </si>
+  <si>
+    <t>ReinstatementMonth</t>
+  </si>
+  <si>
+    <t>Renewable</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Frequencies</t>
+  </si>
+  <si>
+    <t>ContractCurr</t>
+  </si>
+  <si>
+    <t>BillingCurr</t>
+  </si>
+  <si>
+    <t>P0050</t>
+  </si>
+  <si>
+    <t>same_param_item</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>param_datedItem</t>
+  </si>
+  <si>
+    <t>MinSurrMonths</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>arrayName</t>
   </si>
   <si>
-    <t>same_param_item</t>
-  </si>
-  <si>
-    <t>param_datedItem</t>
-  </si>
-  <si>
-    <t>ORDINAL_POSITION</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>FreeLookDays</t>
-  </si>
-  <si>
-    <t>MaxLives</t>
-  </si>
-  <si>
-    <t>Q0005</t>
-  </si>
-  <si>
-    <t>MinLives</t>
-  </si>
-  <si>
-    <t>MinSurrMonths</t>
-  </si>
-  <si>
-    <t>ProductFamily</t>
-  </si>
-  <si>
-    <t>ReinstatementMonth</t>
-  </si>
-  <si>
-    <t>Renewable</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>Frequencies</t>
-  </si>
-  <si>
-    <t>ContractCurr</t>
-  </si>
-  <si>
-    <t>BillingCurr</t>
+    <t>Q0004</t>
+  </si>
+  <si>
+    <t>FREQ</t>
+  </si>
+  <si>
+    <t>CCUR</t>
+  </si>
+  <si>
+    <t>BCUR</t>
+  </si>
+  <si>
+    <t>YESNO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FuturePremAdj         </t>
   </si>
   <si>
     <t>ComponentAddAtAnyTime</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>[4]string</t>
-  </si>
-  <si>
-    <t>[]string</t>
-  </si>
-  <si>
-    <t>Maximum Lives</t>
-  </si>
-  <si>
-    <t>Minimum Lives</t>
-  </si>
-  <si>
-    <t>Contract Currency</t>
-  </si>
-  <si>
-    <t>Billing Currency</t>
-  </si>
-  <si>
-    <t>P0050</t>
-  </si>
-  <si>
-    <t>CCUR</t>
-  </si>
-  <si>
-    <t>BCUR</t>
-  </si>
-  <si>
-    <t>FREQ</t>
-  </si>
-  <si>
-    <t>Free look Days</t>
-  </si>
-  <si>
-    <t>Min.period for Surrender (in months)</t>
-  </si>
-  <si>
-    <t>Product  Family</t>
-  </si>
-  <si>
-    <t>Q0004</t>
-  </si>
-  <si>
-    <t>Reinstatement from PTD (in months)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renewable  </t>
-  </si>
-  <si>
-    <t>YESNO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single </t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Allowable Frequencies</t>
-  </si>
-  <si>
-    <t>Componen tAdd A tAnyTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FuturePremAdj         </t>
-  </si>
-  <si>
     <t>FuturePremAdjYrs</t>
+  </si>
+  <si>
+    <t>[0]string</t>
+  </si>
+  <si>
+    <t>Component Add At AnyTime flag</t>
+  </si>
+  <si>
+    <t>Single life</t>
+  </si>
+  <si>
+    <t>Help_text</t>
+  </si>
+  <si>
+    <t>help_desc</t>
+  </si>
+  <si>
+    <t>Future Premium Adj (in years)</t>
+  </si>
+  <si>
+    <t>Maximum Lives to be included is restricted at 99 lives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Least number of Lives for risk coverage is limited to 1 life </t>
+  </si>
+  <si>
+    <t>Minimum Surrender Period</t>
+  </si>
+  <si>
+    <t>Policy accrues Surrender Value afer 36 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lapsed Policy can be reinstated within 36 months from the date of First Unpaid Premium </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single Premium payment facility as per product features </t>
+  </si>
+  <si>
+    <t>Yearly, Half Yearly, Quarterly and Monthly premium payment amenities are offered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accepted Currencies are INR and USD </t>
+  </si>
+  <si>
+    <t>Billing under INR and USD Currencies are allowed</t>
+  </si>
+  <si>
+    <t>Additional riders, if eligible, could be appended during the term of the policy</t>
+  </si>
+  <si>
+    <t>Free Look cancellation could be effected since policy issuance till 'n' days (both days inclusive)</t>
+  </si>
+  <si>
+    <t>Where ever Future Prem Adj, acceptance is restricted to a maximum of 'n' years .This should be set only when  "Future Premium Adj" flag is set to "Yes".</t>
+  </si>
+  <si>
+    <t>Provision to accept/reject future premia due under the policy. if it is blank or "No", future premium cannot be adjusted for this product.</t>
+  </si>
+  <si>
+    <t>This param table is configured at  product level. For example,  if there are products with product codes AEN, END etc., the parameters for each product are  configured in the respective item in this table. Based on business requirement, multiple dated layers (without overlapping period - from and to dates) can be created for each item.</t>
+  </si>
+  <si>
+    <t>LapsedDays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BillingLeadDays </t>
+  </si>
+  <si>
+    <t>Billing Lead Days (Before Due date)</t>
+  </si>
+  <si>
+    <t>This parameter is configured with the number of days to pay premium after the due date to avoid lapsaton of the policy ; If premium is not paid within this duration (in days), the policy will lapse and the status will be changed to LA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grace period (in Days) </t>
+  </si>
+  <si>
+    <t>This parameter is configured with number of days to generate premium payment notice prior to  the premium due date.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,8 +349,27 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,6 +412,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -284,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -294,12 +441,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -346,7 +506,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,9 +538,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -412,6 +573,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -587,231 +749,268 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="10" max="10" width="24.109375" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="2.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="5" customWidth="1"/>
+    <col min="26" max="26" width="87.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="6"/>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="Z1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="T2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="Z2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="T3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="Z3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="T4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="Z4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="T5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="Z5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>51</v>
@@ -819,354 +1018,430 @@
       <c r="T6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="Z6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="T7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="Z7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="O8" t="s">
         <v>44</v>
       </c>
       <c r="S8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:21">
+      <c r="Z8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="O9" t="s">
         <v>44</v>
       </c>
       <c r="R9" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="S9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="Z9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="O10" t="s">
         <v>44</v>
       </c>
       <c r="S10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="T10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:21">
+      <c r="Z10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="O11" t="s">
         <v>44</v>
       </c>
       <c r="S11" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="T11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="Z11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="O12" t="s">
         <v>44</v>
       </c>
       <c r="R12" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="S12" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="T12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:21">
+      <c r="Z12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I13" s="7"/>
       <c r="J13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="O13" t="s">
         <v>44</v>
       </c>
       <c r="R13" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="S13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="Z13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
         <v>59</v>
       </c>
-      <c r="E14" t="s">
-        <v>23</v>
-      </c>
       <c r="F14" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I14" s="7"/>
       <c r="J14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="O14" t="s">
         <v>44</v>
       </c>
       <c r="R14" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="S14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:21">
+      <c r="Z14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>14</v>
       </c>
-      <c r="D15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
+      <c r="D15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>0</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>20</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I15" s="7"/>
       <c r="J15" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="T15">
         <v>14</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" t="s">
+        <v>84</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="T16">
+        <v>15</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" t="s">
+        <v>82</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="T17">
+        <v>16</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>